<commit_message>
se agrea prototipo sin conexcion y proto con conextion (incrementable)
</commit_message>
<xml_diff>
--- a/samples/demo_clients.xlsx
+++ b/samples/demo_clients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Adri\Universidad\Tesis\Prototipo_reco_datos\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5810CD91-5FCA-4791-A424-BAC0663D3352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C695FB0C-9F12-473A-84AF-CE1B2B8F5263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6075" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{8EA8F648-8439-426B-9DEC-424077CC0F16}"/>
   </bookViews>
@@ -483,6 +483,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>